<commit_message>
Revising tests structure and creating a new test for addressing the issue of optimization with multiple inter-problem sets (currently, endogenous variables are reinitialized every time an inter-problem is solved.
</commit_message>
<xml_diff>
--- a/tests/models/integrated/1_coupled_model/input_data/input_data.xlsx
+++ b/tests/models/integrated/1_coupled_model/input_data/input_data.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\tests\integration\models\5 - coupled_model\input_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\tests\models\integrated\1_coupled_model\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE50F9A-5BE2-47EF-8481-86F99D39DD83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A57BF8F-4962-4238-8C67-6694F9AFD2F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8030" yWindow="2920" windowWidth="20600" windowHeight="15370" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-32840" yWindow="2360" windowWidth="10700" windowHeight="15370" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="x" sheetId="1" r:id="rId1"/>
-    <sheet name="a" sheetId="2" r:id="rId2"/>
+    <sheet name="a" sheetId="2" r:id="rId1"/>
+    <sheet name="x" sheetId="1" r:id="rId2"/>
     <sheet name="products_data" sheetId="3" r:id="rId3"/>
     <sheet name="b" sheetId="4" r:id="rId4"/>
   </sheets>
@@ -23,21 +23,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="15">
   <si>
     <t>id</t>
   </si>
   <si>
+    <t>s_Names</t>
+  </si>
+  <si>
     <t>p_Names</t>
   </si>
   <si>
     <t>values</t>
   </si>
   <si>
+    <t>low energy</t>
+  </si>
+  <si>
     <t>product 1</t>
   </si>
   <si>
     <t>product 2</t>
+  </si>
+  <si>
+    <t>middle energy</t>
+  </si>
+  <si>
+    <t>high energy</t>
   </si>
   <si>
     <t>pd_Names</t>
@@ -417,16 +429,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -436,27 +448,92 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3">
-        <v>20</v>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -465,16 +542,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -484,27 +561,92 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3">
-        <v>10</v>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -517,26 +659,23 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="3" max="3" width="26.08984375" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -544,10 +683,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D2">
         <v>0.9</v>
@@ -558,10 +697,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -572,10 +711,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D4">
         <v>-8.0000000000000002E-3</v>
@@ -586,10 +725,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D5">
         <v>1.2</v>
@@ -600,10 +739,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -614,10 +753,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D7">
         <v>-2E-3</v>
@@ -630,33 +769,67 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4">
         <v>15</v>
       </c>
     </row>

</xml_diff>